<commit_message>
Added Canada source IP
</commit_message>
<xml_diff>
--- a/Domestic.Fraud.Source.IP.xlsx
+++ b/Domestic.Fraud.Source.IP.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-6435" yWindow="2415" windowWidth="17265" windowHeight="4950"/>
+    <workbookView xWindow="195" yWindow="1470" windowWidth="17265" windowHeight="4950"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="74">
   <si>
     <t>Source IP</t>
   </si>
@@ -232,6 +232,12 @@
   </si>
   <si>
     <t xml:space="preserve">91.194.84.60 </t>
+  </si>
+  <si>
+    <t>70.26.209.190</t>
+  </si>
+  <si>
+    <t>Vaureuil, Canada</t>
   </si>
 </sst>
 </file>
@@ -645,10 +651,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B34"/>
+  <dimension ref="A1:B35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="B35" sqref="B35"/>
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="A35" sqref="A35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -919,6 +925,14 @@
       </c>
       <c r="B34" t="s">
         <v>18</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>72</v>
+      </c>
+      <c r="B35" t="s">
+        <v>73</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added IP in China
</commit_message>
<xml_diff>
--- a/Domestic.Fraud.Source.IP.xlsx
+++ b/Domestic.Fraud.Source.IP.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="76">
   <si>
     <t>Source IP</t>
   </si>
@@ -238,6 +238,12 @@
   </si>
   <si>
     <t>Vaureuil, Canada</t>
+  </si>
+  <si>
+    <t>42.2.81.175</t>
+  </si>
+  <si>
+    <t>Hong Kong, China</t>
   </si>
 </sst>
 </file>
@@ -651,10 +657,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B35"/>
+  <dimension ref="A1:B36"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="A35" sqref="A35"/>
+      <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -933,6 +939,14 @@
       </c>
       <c r="B35" t="s">
         <v>73</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>74</v>
+      </c>
+      <c r="B36" t="s">
+        <v>75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added IPs in China, TX, Germany
</commit_message>
<xml_diff>
--- a/Domestic.Fraud.Source.IP.xlsx
+++ b/Domestic.Fraud.Source.IP.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="81">
   <si>
     <t>Source IP</t>
   </si>
@@ -244,6 +244,21 @@
   </si>
   <si>
     <t>Hong Kong, China</t>
+  </si>
+  <si>
+    <t>93.186.202.39</t>
+  </si>
+  <si>
+    <t>158.69.158.67</t>
+  </si>
+  <si>
+    <t>Montreal, Canada</t>
+  </si>
+  <si>
+    <t>23.247.148.238</t>
+  </si>
+  <si>
+    <t>Round Rock, TX</t>
   </si>
 </sst>
 </file>
@@ -657,10 +672,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B36"/>
+  <dimension ref="A1:B39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="B36" sqref="B36"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -935,18 +950,42 @@
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="B35" t="s">
-        <v>73</v>
+        <v>18</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
+        <v>72</v>
+      </c>
+      <c r="B36" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
         <v>74</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B37" t="s">
         <v>75</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>77</v>
+      </c>
+      <c r="B38" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>79</v>
+      </c>
+      <c r="B39" t="s">
+        <v>80</v>
       </c>
     </row>
   </sheetData>

</xml_diff>